<commit_message>
started input user Need sum by date pandas
</commit_message>
<xml_diff>
--- a/excel/test.xlsx
+++ b/excel/test.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna Stray Rongve\Google Drive\Enkeltpersonsforetak\Regnskap\Fakturagenerator\test_registrering\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna Stray Rongve\Google Drive\Enkeltpersonsforetak\Regnskap\Fakturagenerator\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D964B9C2-D115-4AAB-BDBA-62D298E077AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA53B6B-0EB4-4DB7-9B33-F5987956F2F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2170" yWindow="1780" windowWidth="14420" windowHeight="7820" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hour_register" sheetId="1" r:id="rId1"/>
-    <sheet name="1" sheetId="5" r:id="rId2"/>
-    <sheet name="2" sheetId="7" r:id="rId3"/>
-    <sheet name="Students" sheetId="3" r:id="rId4"/>
-    <sheet name="Costumers" sheetId="4" r:id="rId5"/>
-    <sheet name="Company" sheetId="2" r:id="rId6"/>
+    <sheet name="1" sheetId="2" r:id="rId2"/>
+    <sheet name="2" sheetId="3" r:id="rId3"/>
+    <sheet name="Students" sheetId="4" r:id="rId4"/>
+    <sheet name="Costumers" sheetId="5" r:id="rId5"/>
+    <sheet name="Company" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,36 +57,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
-  <si>
-    <t>Anna</t>
-  </si>
-  <si>
-    <t>Hilde</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>rgi</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>hthe</t>
-  </si>
-  <si>
-    <t>24.01.2021</t>
-  </si>
-  <si>
-    <t>REA</t>
-  </si>
-  <si>
-    <t>27.01.2021</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+  <si>
+    <t>Navn</t>
+  </si>
+  <si>
+    <t>Timer</t>
+  </si>
+  <si>
+    <t>Dato</t>
+  </si>
+  <si>
+    <t>Kunde</t>
+  </si>
+  <si>
+    <t>Nora</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Hourly_rate</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Netto</t>
+  </si>
+  <si>
+    <t>MVA</t>
+  </si>
+  <si>
+    <t>MVA_cost</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Undervising</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Anette Evensen</t>
+  </si>
+  <si>
+    <t>anetteengerevensen@gmail.com</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
+    <t>Postalcode</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Kundenummer</t>
+  </si>
+  <si>
+    <t>Realfagspesialisten</t>
+  </si>
+  <si>
+    <t>Kikkutveien 4A</t>
+  </si>
+  <si>
+    <t>0491 Oslo</t>
+  </si>
+  <si>
+    <t>info@realfagspesialisten.com</t>
+  </si>
+  <si>
+    <t>Orgno</t>
+  </si>
+  <si>
+    <t>Account_number</t>
   </si>
   <si>
     <t>Anna Stray Rongve</t>
@@ -105,90 +171,6 @@
   </si>
   <si>
     <t>1506.42.37524</t>
-  </si>
-  <si>
-    <t>Anette Evensen</t>
-  </si>
-  <si>
-    <t>anetteengerevensen@gmail.com</t>
-  </si>
-  <si>
-    <t>Realfagspesialisten</t>
-  </si>
-  <si>
-    <t>Kikkutveien 4A</t>
-  </si>
-  <si>
-    <t>0491 Oslo</t>
-  </si>
-  <si>
-    <t>info@realfagspesialisten.com</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Adress</t>
-  </si>
-  <si>
-    <t>Postalcode</t>
-  </si>
-  <si>
-    <t>Mail</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Account_number</t>
-  </si>
-  <si>
-    <t>Hours</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Costumer</t>
-  </si>
-  <si>
-    <t>Orgno</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Hourly_rate</t>
-  </si>
-  <si>
-    <t>Bonus</t>
-  </si>
-  <si>
-    <t>Netto</t>
-  </si>
-  <si>
-    <t>MVA</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Undervising</t>
-  </si>
-  <si>
-    <t>MVA_cost</t>
-  </si>
-  <si>
-    <t>Kundenummer</t>
   </si>
 </sst>
 </file>
@@ -198,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +201,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -228,7 +215,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -264,12 +251,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -284,10 +286,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
@@ -603,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,161 +623,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>31</v>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44228</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
       </c>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3">
-        <v>44254</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B16">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -780,54 +672,139 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BD4802-D8D7-4DFC-AD49-9342B804C011}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="e" cm="1">
+        <f t="array" ref="B2">SUMPRODUCT((MONTH(hour_register!B:B)=1))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C2">
+        <v>247.5</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="e">
+        <f>B2*C2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2" t="e">
+        <f>E2*F2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H2" t="e">
+        <f>E2+G2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I2" s="3">
+        <v>44228</v>
+      </c>
+      <c r="J2" t="e">
+        <f>H2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" cm="1">
-        <f t="array" ref="B2">SUMPRODUCT((MONTH(hour_register!$C$2:$C$1001)=MONTH(1))*(hour_register!$B$2:$B$1001))</f>
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="B2" t="e" cm="1">
+        <f t="array" ref="B2">MÅNED</f>
+        <v>#NAME?</v>
       </c>
       <c r="C2">
         <v>247.5</v>
@@ -835,111 +812,27 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="e">
         <f>B2*C2</f>
-        <v>3465</v>
-      </c>
-      <c r="F2" s="9">
+        <v>#NAME?</v>
+      </c>
+      <c r="F2" s="8">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="e">
         <f>E2*F2</f>
-        <v>0</v>
-      </c>
-      <c r="H2">
+        <v>#NAME?</v>
+      </c>
+      <c r="H2" t="e">
         <f>E2+G2</f>
-        <v>3465</v>
+        <v>#NAME?</v>
       </c>
       <c r="I2" s="3">
         <v>44228</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2" t="e">
         <f>H2</f>
-        <v>3465</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E101A67-FF19-4B49-BCE2-732349B93EA3}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" cm="1">
-        <f t="array" ref="B2">SUMPRODUCT((MONTH(hour_register!$C$2:$C$1001)=MONTH(hour_register!C2&amp;2))*(hour_register!$B$2:$B$1001))</f>
-        <v>14</v>
-      </c>
-      <c r="C2">
-        <v>247.5</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f>B2*C2</f>
-        <v>3465</v>
-      </c>
-      <c r="F2" s="9">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <f>E2*F2</f>
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <f>E2+G2</f>
-        <v>3465</v>
-      </c>
-      <c r="I2" s="3">
-        <v>44228</v>
-      </c>
-      <c r="J2" s="2">
-        <f>H2</f>
-        <v>3465</v>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
@@ -948,7 +841,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA0AAA5-3F77-4387-A206-3AFDA3DF0199}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -959,13 +852,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -973,10 +866,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>95338955</v>
@@ -984,18 +877,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{A9D03BDB-B774-478A-99AD-38A94F565E6D}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF65E71A-106C-4596-A5DD-DB20503D05E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1010,22 +905,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1033,16 +928,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G2">
         <f>A2+1</f>
@@ -1055,7 +950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B47113-3865-4936-A7A3-021E9D2BD7B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1072,25 +967,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1098,25 +993,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G2">
         <v>924881682</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>